<commit_message>
Caresens Beta quality library checkin, and an updated meterlist
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t xml:space="preserve">Abbott Laboratories </t>
   </si>
@@ -117,9 +117,6 @@
     <t>Contour *</t>
   </si>
   <si>
-    <t>Caresens-N *</t>
-  </si>
-  <si>
     <t>OneTouch UltraMini *</t>
   </si>
   <si>
@@ -205,6 +202,30 @@
   </si>
   <si>
     <t>OneTouch Ultra</t>
+  </si>
+  <si>
+    <t>Caresens N *</t>
+  </si>
+  <si>
+    <t>Caresens N POP</t>
+  </si>
+  <si>
+    <t>Caresens N Mini</t>
+  </si>
+  <si>
+    <t>Caresens N Voice</t>
+  </si>
+  <si>
+    <t>Caresens II</t>
+  </si>
+  <si>
+    <t>Caresens POP</t>
+  </si>
+  <si>
+    <t>COOL</t>
+  </si>
+  <si>
+    <t>alphacheck professional</t>
   </si>
 </sst>
 </file>
@@ -350,7 +371,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -368,6 +389,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -676,7 +699,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +710,7 @@
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -722,19 +745,19 @@
         <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
+      <c r="G2" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -756,13 +779,16 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>23</v>
@@ -775,6 +801,9 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -785,16 +814,19 @@
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,13 +837,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -819,12 +854,23 @@
         <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -840,7 +886,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -848,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -856,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -864,12 +910,12 @@
         <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>20</v>
@@ -900,35 +946,35 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>2303</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>451</v>
@@ -937,24 +983,24 @@
         <v>3410</v>
       </c>
       <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>6001</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added space below grid to prevent overlapping on tablets
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
@@ -90,9 +90,6 @@
     <t>OneTouch Ultra Smart *</t>
   </si>
   <si>
-    <t>Accu Chek Aviva Nano *</t>
-  </si>
-  <si>
     <t>TRUEtrack *</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>alphacheck professional</t>
+  </si>
+  <si>
+    <t>Accu Chek Aviva Nano</t>
   </si>
 </sst>
 </file>
@@ -699,7 +699,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,27 +742,27 @@
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -771,7 +771,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -780,7 +780,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -788,89 +788,89 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -886,7 +886,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -910,12 +910,12 @@
         <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>20</v>
@@ -946,35 +946,35 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>2303</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>451</v>
@@ -983,24 +983,24 @@
         <v>3410</v>
       </c>
       <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>6001</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed main graph color, and updated meter list
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
@@ -225,7 +225,7 @@
     <t>alphacheck professional</t>
   </si>
   <si>
-    <t>Accu Chek Aviva Nano</t>
+    <t>Accu Chek Aviva Nano*</t>
   </si>
 </sst>
 </file>
@@ -389,8 +389,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +756,7 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>61</v>
       </c>
     </row>
@@ -802,7 +802,7 @@
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>63</v>
       </c>
     </row>
@@ -856,7 +856,7 @@
       <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial Contour USB check-in.  Header records reading and parsed.
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t xml:space="preserve">Abbott Laboratories </t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Accu Chek Aviva Nano*</t>
+  </si>
+  <si>
+    <t>Contour Next USB*</t>
+  </si>
+  <si>
+    <t>Contour Next EZ*</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -391,6 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -699,7 +706,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +817,7 @@
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -853,6 +860,9 @@
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
@@ -861,6 +871,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Final check-in for Contour_USB, webservice tweaks to get it working again, added code to distinguish Contour USB and Contour USB Next in the database to help finer granulate data.
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbarnhill\Desktop\Dropbox\Projects\GlucaTrack\GlucaTrack.Communication\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -397,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -411,6 +416,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -459,7 +467,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,7 +502,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -706,7 +714,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +825,7 @@
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -860,7 +868,7 @@
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E7" s="2" t="s">

</xml_diff>

<commit_message>
Updated supported meters document
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t xml:space="preserve">Abbott Laboratories </t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Contour Next EZ*</t>
+  </si>
+  <si>
+    <t>Contour Next*</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -403,6 +406,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -714,7 +718,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +883,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>71</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -890,6 +894,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
reassigned new keys to each project, installer work to start notify icon on install.  Still lacks stopping notify icon on uninstall and background of launch now checkmark background.
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbarnhill\Desktop\Dropbox\Projects\GlucaTrack\GlucaTrack.Communication\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meters" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t xml:space="preserve">Abbott Laboratories </t>
   </si>
@@ -50,9 +45,6 @@
     <t xml:space="preserve">AgaMatrix </t>
   </si>
   <si>
-    <t>Accu Chek Compact Plus</t>
-  </si>
-  <si>
     <t>WaveSense Jazz</t>
   </si>
   <si>
@@ -240,6 +232,15 @@
   </si>
   <si>
     <t>Contour Next*</t>
+  </si>
+  <si>
+    <t>Accu Chek Compact Plus*</t>
+  </si>
+  <si>
+    <t>Contour USB</t>
+  </si>
+  <si>
+    <t>Contour USB Next</t>
   </si>
 </sst>
 </file>
@@ -471,7 +472,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -506,7 +507,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +727,7 @@
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
@@ -753,53 +754,53 @@
         <v>8</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -807,146 +808,146 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -957,10 +958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,35 +975,35 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>2303</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>451</v>
@@ -1011,24 +1012,38 @@
         <v>3410</v>
       </c>
       <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4">
-        <v>6001</v>
+        <v>6002</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5">
+        <v>7410</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added download page, added supported meters page and link on main page, webservice returns list of supported meters, updated meters document
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbarnhill\Desktop\Dropbox\Projects\GlucaTrack\GlucaTrack.Communication\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Meters" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t xml:space="preserve">Abbott Laboratories </t>
   </si>
@@ -241,6 +246,9 @@
   </si>
   <si>
     <t>Contour USB Next</t>
+  </si>
+  <si>
+    <t>OneTouch Verio IQ</t>
   </si>
 </sst>
 </file>
@@ -472,7 +480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,7 +515,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -718,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +884,9 @@
       <c r="B7" s="17" t="s">
         <v>69</v>
       </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
@@ -960,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modied WIX installer to close notify icon on uninstall, updated EULA with some minor changes and corrections, updated the meter list,
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t xml:space="preserve">Abbott Laboratories </t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>OneTouch Verio IQ</t>
+  </si>
+  <si>
+    <t>OneTouch Ping</t>
   </si>
 </sst>
 </file>
@@ -726,7 +729,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +863,7 @@
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -896,6 +899,9 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added ability to switch notify icons from enabled to disabled and busy.  Busy icon still needs to be created but only replace what is in the resources.
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbarnhill\Desktop\Dropbox\Projects\GlucaTrack\GlucaTrack.Communication\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -32,12 +27,6 @@
     <t xml:space="preserve">LifeScan </t>
   </si>
   <si>
-    <t>Contour TS</t>
-  </si>
-  <si>
-    <t>Precision Xtra</t>
-  </si>
-  <si>
     <t>Bayer Didget</t>
   </si>
   <si>
@@ -53,9 +42,6 @@
     <t>WaveSense Jazz</t>
   </si>
   <si>
-    <t>TRUEresult</t>
-  </si>
-  <si>
     <t>WaveSense Presto</t>
   </si>
   <si>
@@ -200,9 +186,6 @@
     <t>Bayer Health Care LLC</t>
   </si>
   <si>
-    <t>OneTouch Ultra</t>
-  </si>
-  <si>
     <t>Caresens N *</t>
   </si>
   <si>
@@ -252,6 +235,18 @@
   </si>
   <si>
     <t>OneTouch Ping</t>
+  </si>
+  <si>
+    <t>OneTouch Ultra*</t>
+  </si>
+  <si>
+    <t>Contour TS*</t>
+  </si>
+  <si>
+    <t>Precision Xtra*</t>
+  </si>
+  <si>
+    <t>TRUEresult*</t>
   </si>
 </sst>
 </file>
@@ -342,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -389,6 +384,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -397,7 +416,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -415,9 +434,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -482,7 +506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,7 +541,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -729,241 +753,250 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>19</v>
+      <c r="G1" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
+        <v>68</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>60</v>
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>4</v>
+      <c r="A4" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
+      <c r="B8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>71</v>
-      </c>
+      <c r="B9" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -991,35 +1024,35 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>2303</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>451</v>
@@ -1028,38 +1061,38 @@
         <v>3410</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>6002</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>7410</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited supported meter document
</commit_message>
<xml_diff>
--- a/GlucaTrack.Communication/Documents/MeterList.xlsx
+++ b/GlucaTrack.Communication/Documents/MeterList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbarnhill\Desktop\Dropbox\Projects\GlucaTrack\GlucaTrack.Communication\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -506,7 +511,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,7 +546,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -753,7 +758,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +895,7 @@
       <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="2" t="s">

</xml_diff>